<commit_message>
update script database xlsx
</commit_message>
<xml_diff>
--- a/r0 SCRIPTS.xlsx
+++ b/r0 SCRIPTS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanfeishen/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josh.buser\Documents\GitHub\cd-alpha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66F5154F-524D-1B4F-9E5A-9C3A45D9C4FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25845D05-165D-4F7B-B950-759F2EC2CD7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4520" yWindow="2240" windowWidth="24280" windowHeight="13780" xr2:uid="{4F228711-34F2-CD4A-B88C-4A9EDC5CE2D1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4F228711-34F2-CD4A-B88C-4A9EDC5CE2D1}"/>
   </bookViews>
   <sheets>
     <sheet name="r0" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="93">
   <si>
     <t>Sample Flow Rate</t>
   </si>
@@ -302,6 +302,18 @@
   </si>
   <si>
     <t>Hanfei's flow rate optimization</t>
+  </si>
+  <si>
+    <t>ExoT_r0_script_8v0</t>
+  </si>
+  <si>
+    <t>ExoT_r0_script_8v1</t>
+  </si>
+  <si>
+    <t>ExoT_r0_script_8v2</t>
+  </si>
+  <si>
+    <t>ExoT_r0_script_8v3</t>
   </si>
 </sst>
 </file>
@@ -693,31 +705,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{865254A0-CD44-564E-904D-D988B38D1DFE}">
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.19921875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="49" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.69921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.19921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.69921875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.69921875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="20.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -752,7 +767,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -787,7 +802,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -822,7 +837,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -857,7 +872,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -892,7 +907,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>65</v>
       </c>
@@ -927,7 +942,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>66</v>
       </c>
@@ -962,7 +977,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>67</v>
       </c>
@@ -997,7 +1012,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>68</v>
       </c>
@@ -1032,7 +1047,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>69</v>
       </c>
@@ -1067,7 +1082,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>74</v>
       </c>
@@ -1102,7 +1117,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>77</v>
       </c>
@@ -1137,7 +1152,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>79</v>
       </c>
@@ -1172,7 +1187,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>80</v>
       </c>
@@ -1207,7 +1222,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>82</v>
       </c>
@@ -1239,7 +1254,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>83</v>
       </c>
@@ -1274,7 +1289,80 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" t="s">
+        <v>87</v>
+      </c>
+      <c r="H19" t="s">
+        <v>14</v>
+      </c>
+      <c r="I19" t="s">
+        <v>28</v>
+      </c>
+      <c r="J19" t="s">
+        <v>23</v>
+      </c>
+      <c r="K19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>90</v>
+      </c>
+      <c r="B20" t="s">
+        <v>88</v>
+      </c>
+      <c r="C20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" t="s">
+        <v>71</v>
+      </c>
+      <c r="H20" t="s">
+        <v>14</v>
+      </c>
+      <c r="I20" t="s">
+        <v>28</v>
+      </c>
+      <c r="J20" t="s">
+        <v>23</v>
+      </c>
+      <c r="K20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>91</v>
+      </c>
       <c r="B21" t="s">
         <v>88</v>
       </c>
@@ -1291,7 +1379,7 @@
         <v>20</v>
       </c>
       <c r="G21" t="s">
-        <v>87</v>
+        <v>15</v>
       </c>
       <c r="H21" t="s">
         <v>14</v>
@@ -1306,7 +1394,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>92</v>
+      </c>
       <c r="B22" t="s">
         <v>88</v>
       </c>
@@ -1323,7 +1414,7 @@
         <v>20</v>
       </c>
       <c r="G22" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H22" t="s">
         <v>14</v>
@@ -1335,70 +1426,6 @@
         <v>23</v>
       </c>
       <c r="K22" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B23" t="s">
-        <v>88</v>
-      </c>
-      <c r="C23" t="s">
-        <v>13</v>
-      </c>
-      <c r="D23" t="s">
-        <v>12</v>
-      </c>
-      <c r="E23" t="s">
-        <v>30</v>
-      </c>
-      <c r="F23" t="s">
-        <v>20</v>
-      </c>
-      <c r="G23" t="s">
-        <v>15</v>
-      </c>
-      <c r="H23" t="s">
-        <v>14</v>
-      </c>
-      <c r="I23" t="s">
-        <v>28</v>
-      </c>
-      <c r="J23" t="s">
-        <v>23</v>
-      </c>
-      <c r="K23" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" t="s">
-        <v>88</v>
-      </c>
-      <c r="C24" t="s">
-        <v>13</v>
-      </c>
-      <c r="D24" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" t="s">
-        <v>30</v>
-      </c>
-      <c r="F24" t="s">
-        <v>20</v>
-      </c>
-      <c r="G24" t="s">
-        <v>72</v>
-      </c>
-      <c r="H24" t="s">
-        <v>14</v>
-      </c>
-      <c r="I24" t="s">
-        <v>28</v>
-      </c>
-      <c r="J24" t="s">
-        <v>23</v>
-      </c>
-      <c r="K24" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1416,20 +1443,20 @@
       <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" customWidth="1"/>
-    <col min="2" max="2" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.796875" customWidth="1"/>
+    <col min="2" max="2" width="43.69921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.69921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.19921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.796875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.69921875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.69921875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>85</v>
       </c>
@@ -1444,7 +1471,7 @@
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1479,7 +1506,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>86</v>
       </c>
@@ -1527,14 +1554,14 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="50" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -1542,7 +1569,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1550,10 +1577,10 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>41</v>
       </c>
@@ -1561,7 +1588,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>42</v>
       </c>
@@ -1569,10 +1596,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>36</v>
       </c>
@@ -1586,7 +1613,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1597,7 +1624,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1611,7 +1638,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>3</v>
       </c>
@@ -1625,7 +1652,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>4</v>
       </c>
@@ -1640,7 +1667,7 @@
       </c>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>5</v>
       </c>
@@ -1654,7 +1681,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>6</v>
       </c>
@@ -1668,7 +1695,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>7</v>
       </c>
@@ -1682,7 +1709,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>8</v>
       </c>
@@ -1696,7 +1723,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>9</v>
       </c>
@@ -1710,7 +1737,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>10</v>
       </c>
@@ -1724,7 +1751,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>11</v>
       </c>
@@ -1738,7 +1765,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
update for andrews 5ml/hr exps
</commit_message>
<xml_diff>
--- a/r0 SCRIPTS.xlsx
+++ b/r0 SCRIPTS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanfeishen/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josh.buser\Documents\GitHub\cd-alpha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2B8CA0C-A8E2-3D49-8353-58C1B110F1D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B22C9B82-EA6C-4E90-80CC-86EA303760FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2520" yWindow="460" windowWidth="23260" windowHeight="12580" xr2:uid="{4F228711-34F2-CD4A-B88C-4A9EDC5CE2D1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4F228711-34F2-CD4A-B88C-4A9EDC5CE2D1}"/>
   </bookViews>
   <sheets>
     <sheet name="r0" sheetId="1" r:id="rId1"/>
@@ -316,10 +316,10 @@
     <t>ExoT_r0_script_8v3</t>
   </si>
   <si>
-    <t>ExoT_r0_script_9v1</t>
-  </si>
-  <si>
     <t>Andrew Lin 081120</t>
+  </si>
+  <si>
+    <t>ExoT_r0_script_9v0</t>
   </si>
 </sst>
 </file>
@@ -714,31 +714,31 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="H23" sqref="H23"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4:XFD23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.19921875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="49" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.69921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.19921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.69921875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.69921875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="20.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -773,7 +773,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -808,7 +808,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -843,7 +843,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -878,7 +878,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -913,7 +913,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>65</v>
       </c>
@@ -948,7 +948,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>66</v>
       </c>
@@ -983,7 +983,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>67</v>
       </c>
@@ -1018,7 +1018,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>68</v>
       </c>
@@ -1053,7 +1053,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>69</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>74</v>
       </c>
@@ -1123,7 +1123,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>77</v>
       </c>
@@ -1158,7 +1158,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>79</v>
       </c>
@@ -1193,7 +1193,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>80</v>
       </c>
@@ -1228,7 +1228,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>82</v>
       </c>
@@ -1260,7 +1260,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>83</v>
       </c>
@@ -1295,7 +1295,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>89</v>
       </c>
@@ -1330,7 +1330,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>90</v>
       </c>
@@ -1365,7 +1365,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>91</v>
       </c>
@@ -1400,7 +1400,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>92</v>
       </c>
@@ -1435,12 +1435,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>94</v>
+      </c>
+      <c r="B23" t="s">
         <v>93</v>
-      </c>
-      <c r="B23" t="s">
-        <v>94</v>
       </c>
       <c r="C23" t="s">
         <v>12</v>
@@ -1484,20 +1484,20 @@
       <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" customWidth="1"/>
-    <col min="2" max="2" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.796875" customWidth="1"/>
+    <col min="2" max="2" width="43.69921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.69921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.19921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.796875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.69921875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.69921875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>85</v>
       </c>
@@ -1512,7 +1512,7 @@
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1547,7 +1547,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>86</v>
       </c>
@@ -1595,14 +1595,14 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="50" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -1610,7 +1610,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1618,10 +1618,10 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>41</v>
       </c>
@@ -1629,7 +1629,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>42</v>
       </c>
@@ -1637,10 +1637,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>36</v>
       </c>
@@ -1654,7 +1654,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1665,7 +1665,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1679,7 +1679,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>3</v>
       </c>
@@ -1693,7 +1693,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>4</v>
       </c>
@@ -1708,7 +1708,7 @@
       </c>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>5</v>
       </c>
@@ -1722,7 +1722,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>6</v>
       </c>
@@ -1736,7 +1736,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>7</v>
       </c>
@@ -1750,7 +1750,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>8</v>
       </c>
@@ -1764,7 +1764,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>9</v>
       </c>
@@ -1778,7 +1778,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>10</v>
       </c>
@@ -1792,7 +1792,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>11</v>
       </c>
@@ -1806,7 +1806,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
create 1v1 for seq exps
</commit_message>
<xml_diff>
--- a/r0 SCRIPTS.xlsx
+++ b/r0 SCRIPTS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josh.buser\Documents\GitHub\cd-alpha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5738A81-88EE-4CB5-9D31-A43A6E51E5F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8089F3E1-EA41-46A8-8E2B-0A77287F7BC0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1116" yWindow="1116" windowWidth="16584" windowHeight="8964" xr2:uid="{4F228711-34F2-CD4A-B88C-4A9EDC5CE2D1}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="16584" windowHeight="8964" xr2:uid="{4F228711-34F2-CD4A-B88C-4A9EDC5CE2D1}"/>
   </bookViews>
   <sheets>
     <sheet name="r0" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="107">
   <si>
     <t>Sample Flow Rate</t>
   </si>
@@ -347,6 +347,15 @@
   </si>
   <si>
     <t>1200-1200-1200-1200-1200-1200</t>
+  </si>
+  <si>
+    <t>ExoT_r0_script_1v1</t>
+  </si>
+  <si>
+    <t>Lung Cancer Clinical Study (1 mL plasma sample)</t>
+  </si>
+  <si>
+    <t>1.0 mL</t>
   </si>
 </sst>
 </file>
@@ -738,13 +747,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{865254A0-CD44-564E-904D-D988B38D1DFE}">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A30" sqref="A30"/>
+      <selection pane="bottomRight" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -837,13 +846,13 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>104</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>105</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -852,7 +861,7 @@
         <v>30</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>106</v>
       </c>
       <c r="G5" t="s">
         <v>14</v>
@@ -872,10 +881,10 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
@@ -887,7 +896,7 @@
         <v>30</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G6" t="s">
         <v>14</v>
@@ -907,10 +916,10 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C7" t="s">
         <v>13</v>
@@ -922,30 +931,30 @@
         <v>30</v>
       </c>
       <c r="F7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H7" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7">
-        <v>1000</v>
+        <v>14</v>
+      </c>
+      <c r="I7" t="s">
+        <v>28</v>
       </c>
       <c r="J7" t="s">
         <v>23</v>
       </c>
       <c r="K7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
         <v>13</v>
@@ -960,24 +969,24 @@
         <v>21</v>
       </c>
       <c r="G8" t="s">
-        <v>71</v>
+        <v>15</v>
       </c>
       <c r="H8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I8" t="s">
-        <v>28</v>
+        <v>15</v>
+      </c>
+      <c r="I8">
+        <v>1000</v>
       </c>
       <c r="J8" t="s">
         <v>23</v>
       </c>
       <c r="K8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B9" t="s">
         <v>70</v>
@@ -995,7 +1004,7 @@
         <v>21</v>
       </c>
       <c r="G9" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="H9" t="s">
         <v>14</v>
@@ -1012,7 +1021,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B10" t="s">
         <v>70</v>
@@ -1030,7 +1039,7 @@
         <v>21</v>
       </c>
       <c r="G10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H10" t="s">
         <v>14</v>
@@ -1047,7 +1056,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B11" t="s">
         <v>70</v>
@@ -1065,7 +1074,7 @@
         <v>21</v>
       </c>
       <c r="G11" t="s">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="H11" t="s">
         <v>14</v>
@@ -1082,7 +1091,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B12" t="s">
         <v>70</v>
@@ -1100,7 +1109,7 @@
         <v>21</v>
       </c>
       <c r="G12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H12" t="s">
         <v>14</v>
@@ -1117,13 +1126,13 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B13" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D13" t="s">
         <v>12</v>
@@ -1132,10 +1141,10 @@
         <v>30</v>
       </c>
       <c r="F13" t="s">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="G13" t="s">
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="H13" t="s">
         <v>14</v>
@@ -1152,13 +1161,13 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B14" t="s">
         <v>75</v>
       </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D14" t="s">
         <v>12</v>
@@ -1187,10 +1196,10 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B15" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C15" t="s">
         <v>13</v>
@@ -1202,7 +1211,7 @@
         <v>30</v>
       </c>
       <c r="F15" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="G15" t="s">
         <v>14</v>
@@ -1222,13 +1231,13 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B16" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C16" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D16" t="s">
         <v>12</v>
@@ -1237,7 +1246,7 @@
         <v>30</v>
       </c>
       <c r="F16" t="s">
-        <v>76</v>
+        <v>20</v>
       </c>
       <c r="G16" t="s">
         <v>14</v>
@@ -1257,7 +1266,10 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>82</v>
+        <v>80</v>
+      </c>
+      <c r="B17" t="s">
+        <v>81</v>
       </c>
       <c r="C17" t="s">
         <v>12</v>
@@ -1289,10 +1301,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>83</v>
-      </c>
-      <c r="B18" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C18" t="s">
         <v>12</v>
@@ -1324,13 +1333,13 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B19" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D19" t="s">
         <v>12</v>
@@ -1339,10 +1348,10 @@
         <v>30</v>
       </c>
       <c r="F19" t="s">
-        <v>20</v>
+        <v>76</v>
       </c>
       <c r="G19" t="s">
-        <v>87</v>
+        <v>14</v>
       </c>
       <c r="H19" t="s">
         <v>14</v>
@@ -1359,7 +1368,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B20" t="s">
         <v>88</v>
@@ -1377,7 +1386,7 @@
         <v>20</v>
       </c>
       <c r="G20" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
       <c r="H20" t="s">
         <v>14</v>
@@ -1394,7 +1403,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B21" t="s">
         <v>88</v>
@@ -1412,7 +1421,7 @@
         <v>20</v>
       </c>
       <c r="G21" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="H21" t="s">
         <v>14</v>
@@ -1427,9 +1436,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B22" t="s">
         <v>88</v>
@@ -1447,7 +1456,7 @@
         <v>20</v>
       </c>
       <c r="G22" t="s">
-        <v>72</v>
+        <v>15</v>
       </c>
       <c r="H22" t="s">
         <v>14</v>
@@ -1462,15 +1471,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B23" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C23" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D23" t="s">
         <v>12</v>
@@ -1479,13 +1488,13 @@
         <v>30</v>
       </c>
       <c r="F23" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G23" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H23" t="s">
-        <v>71</v>
+        <v>14</v>
       </c>
       <c r="I23" t="s">
         <v>28</v>
@@ -1499,13 +1508,13 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B24" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D24" t="s">
         <v>12</v>
@@ -1514,16 +1523,16 @@
         <v>30</v>
       </c>
       <c r="F24" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G24" t="s">
-        <v>14</v>
+        <v>71</v>
       </c>
       <c r="H24" t="s">
-        <v>14</v>
+        <v>71</v>
       </c>
       <c r="I24" t="s">
-        <v>97</v>
+        <v>28</v>
       </c>
       <c r="J24" t="s">
         <v>23</v>
@@ -1534,7 +1543,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B25" t="s">
         <v>96</v>
@@ -1558,7 +1567,7 @@
         <v>14</v>
       </c>
       <c r="I25" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="J25" t="s">
         <v>23</v>
@@ -1569,7 +1578,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B26" t="s">
         <v>96</v>
@@ -1593,7 +1602,7 @@
         <v>14</v>
       </c>
       <c r="I26" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J26" t="s">
         <v>23</v>
@@ -1604,7 +1613,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B27" t="s">
         <v>96</v>
@@ -1628,12 +1637,47 @@
         <v>14</v>
       </c>
       <c r="I27" t="s">
+        <v>101</v>
+      </c>
+      <c r="J27" t="s">
+        <v>23</v>
+      </c>
+      <c r="K27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>102</v>
+      </c>
+      <c r="B28" t="s">
+        <v>96</v>
+      </c>
+      <c r="C28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" t="s">
+        <v>30</v>
+      </c>
+      <c r="F28" t="s">
+        <v>20</v>
+      </c>
+      <c r="G28" t="s">
+        <v>14</v>
+      </c>
+      <c r="H28" t="s">
+        <v>14</v>
+      </c>
+      <c r="I28" t="s">
         <v>103</v>
       </c>
-      <c r="J27" t="s">
-        <v>23</v>
-      </c>
-      <c r="K27" t="s">
+      <c r="J28" t="s">
+        <v>23</v>
+      </c>
+      <c r="K28" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added v0 scripts for western blot
2v0, 3v0 to test change lysis pull to waste syringe first
</commit_message>
<xml_diff>
--- a/r0 SCRIPTS.xlsx
+++ b/r0 SCRIPTS.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chipdx/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E863FF87-3105-054D-8BF4-FFAFE7A4623E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3467921-0331-F24E-9AE7-AF57A8528615}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="900" windowWidth="25480" windowHeight="15100" xr2:uid="{4F228711-34F2-CD4A-B88C-4A9EDC5CE2D1}"/>
+    <workbookView xWindow="120" yWindow="900" windowWidth="25480" windowHeight="15100" activeTab="1" xr2:uid="{4F228711-34F2-CD4A-B88C-4A9EDC5CE2D1}"/>
   </bookViews>
   <sheets>
     <sheet name="r0" sheetId="1" r:id="rId1"/>
     <sheet name="v0" sheetId="3" r:id="rId2"/>
     <sheet name="1v0" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029" iterateCount="1"/>
+  <calcPr calcId="191029" iterateCount="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,6 +28,7 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="116">
   <si>
     <t>Sample Flow Rate</t>
   </si>
@@ -365,6 +366,24 @@
   </si>
   <si>
     <t>2 mL plasma sample- Quant-iT</t>
+  </si>
+  <si>
+    <t>v0_script_2v0</t>
+  </si>
+  <si>
+    <t>Western Blot 1</t>
+  </si>
+  <si>
+    <t>Western Blot 1 - change lysis pull to waste syringe</t>
+  </si>
+  <si>
+    <t>v0_script_3v0</t>
+  </si>
+  <si>
+    <t>5 mins (RIPA - 500 uL)</t>
+  </si>
+  <si>
+    <t>***CHANGE FROM 1V0: after add RIPA lysis buffer, pull to WASTE syringe first, 5 min incubation, then LAST pull to LYSATE syringe (test with dyes, may need to increase pull to 700 uL to match QIAzol since this gets lysis buffer to outlet of chip, but may leave reservoir empty, affect last pull?)</t>
   </si>
 </sst>
 </file>
@@ -416,12 +435,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -436,12 +461,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -758,8 +784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{865254A0-CD44-564E-904D-D988B38D1DFE}">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="C30" sqref="C30"/>
@@ -1733,10 +1759,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{789722DC-7BCB-4884-BC3A-D96FA1424135}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1752,7 +1778,7 @@
     <col min="11" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>85</v>
       </c>
@@ -1767,7 +1793,7 @@
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1801,8 +1827,9 @@
       <c r="K3" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="N3" s="1"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>86</v>
       </c>
@@ -1835,6 +1862,79 @@
       </c>
       <c r="K4" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>110</v>
+      </c>
+      <c r="B5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="K5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="K6" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" s="5" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added 4v0(demo) and 5v0(panc)
</commit_message>
<xml_diff>
--- a/r0 SCRIPTS.xlsx
+++ b/r0 SCRIPTS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chipdx/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josh.buser\Documents\GitHub\cd-alpha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3467921-0331-F24E-9AE7-AF57A8528615}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6375953A-0BC9-4F7C-AC69-ECD837DE7105}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="900" windowWidth="25480" windowHeight="15100" activeTab="1" xr2:uid="{4F228711-34F2-CD4A-B88C-4A9EDC5CE2D1}"/>
+    <workbookView xWindow="6456" yWindow="3396" windowWidth="16584" windowHeight="8964" activeTab="1" xr2:uid="{4F228711-34F2-CD4A-B88C-4A9EDC5CE2D1}"/>
   </bookViews>
   <sheets>
     <sheet name="r0" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="125">
   <si>
     <t>Sample Flow Rate</t>
   </si>
@@ -384,13 +384,40 @@
   </si>
   <si>
     <t>***CHANGE FROM 1V0: after add RIPA lysis buffer, pull to WASTE syringe first, 5 min incubation, then LAST pull to LYSATE syringe (test with dyes, may need to increase pull to 700 uL to match QIAzol since this gets lysis buffer to outlet of chip, but may leave reservoir empty, affect last pull?)</t>
+  </si>
+  <si>
+    <t>v0-protocol-4v0.json</t>
+  </si>
+  <si>
+    <t>LC - short waits for demo</t>
+  </si>
+  <si>
+    <t>15 sec</t>
+  </si>
+  <si>
+    <t>PANC 1.5 mL Plasma (Yang CCR 2020)</t>
+  </si>
+  <si>
+    <t>1.5 mL</t>
+  </si>
+  <si>
+    <t>1.5 mL/hr</t>
+  </si>
+  <si>
+    <t>3 mins (QIAZOL - 700 uL)</t>
+  </si>
+  <si>
+    <t>Pull 700 uL to WASTE SYRINGE, 3 min incubation, then final pull to lysate syringe</t>
+  </si>
+  <si>
+    <t>v0-protocol-5v0.json</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -434,6 +461,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -461,13 +495,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -785,31 +823,31 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.19921875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="49" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.69921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.19921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.69921875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.69921875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="20.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -844,7 +882,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -879,7 +917,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>104</v>
       </c>
@@ -914,7 +952,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -949,7 +987,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -984,7 +1022,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1019,7 +1057,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>65</v>
       </c>
@@ -1054,7 +1092,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>66</v>
       </c>
@@ -1089,7 +1127,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>67</v>
       </c>
@@ -1124,7 +1162,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -1159,7 +1197,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>69</v>
       </c>
@@ -1194,7 +1232,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>74</v>
       </c>
@@ -1229,7 +1267,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>77</v>
       </c>
@@ -1264,7 +1302,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>79</v>
       </c>
@@ -1299,7 +1337,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>80</v>
       </c>
@@ -1334,7 +1372,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>82</v>
       </c>
@@ -1366,7 +1404,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>83</v>
       </c>
@@ -1401,7 +1439,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>89</v>
       </c>
@@ -1436,7 +1474,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>90</v>
       </c>
@@ -1471,7 +1509,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>91</v>
       </c>
@@ -1506,7 +1544,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>92</v>
       </c>
@@ -1541,7 +1579,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>94</v>
       </c>
@@ -1576,7 +1614,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>95</v>
       </c>
@@ -1611,7 +1649,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>98</v>
       </c>
@@ -1646,7 +1684,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>100</v>
       </c>
@@ -1681,7 +1719,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>102</v>
       </c>
@@ -1716,7 +1754,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>108</v>
       </c>
@@ -1759,26 +1797,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{789722DC-7BCB-4884-BC3A-D96FA1424135}">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" customWidth="1"/>
-    <col min="2" max="2" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.796875" customWidth="1"/>
+    <col min="2" max="2" width="43.69921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.69921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.19921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.796875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.69921875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.69921875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>85</v>
       </c>
@@ -1793,7 +1831,7 @@
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1829,7 +1867,7 @@
       </c>
       <c r="N3" s="1"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>86</v>
       </c>
@@ -1864,7 +1902,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>110</v>
       </c>
@@ -1899,7 +1937,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>113</v>
       </c>
@@ -1935,6 +1973,79 @@
       </c>
       <c r="L6" s="5" t="s">
         <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>116</v>
+      </c>
+      <c r="B7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>118</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7">
+        <v>500</v>
+      </c>
+      <c r="J7" t="s">
+        <v>118</v>
+      </c>
+      <c r="K7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F8" t="s">
+        <v>120</v>
+      </c>
+      <c r="G8" t="s">
+        <v>121</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="I8" s="7">
+        <v>1000</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="K8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L8" s="5" t="s">
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1950,14 +2061,14 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="50" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -1965,7 +2076,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1973,10 +2084,10 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>41</v>
       </c>
@@ -1984,7 +2095,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>42</v>
       </c>
@@ -1992,10 +2103,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>36</v>
       </c>
@@ -2009,7 +2120,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2020,7 +2131,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2</v>
       </c>
@@ -2034,7 +2145,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>3</v>
       </c>
@@ -2048,7 +2159,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>4</v>
       </c>
@@ -2063,7 +2174,7 @@
       </c>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>5</v>
       </c>
@@ -2077,7 +2188,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>6</v>
       </c>
@@ -2091,7 +2202,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>7</v>
       </c>
@@ -2105,7 +2216,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>8</v>
       </c>
@@ -2119,7 +2230,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>9</v>
       </c>
@@ -2133,7 +2244,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>10</v>
       </c>
@@ -2147,7 +2258,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>11</v>
       </c>
@@ -2161,7 +2272,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
update script log for 12vX immune flow rate opt
</commit_message>
<xml_diff>
--- a/r0 SCRIPTS.xlsx
+++ b/r0 SCRIPTS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chipdx/Documents/Protocols/r0 and v0 SCRIPT PROTOCOLS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josh.buser\Documents\GitHub\cd-alpha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6FA8DEB-4620-7F49-B478-A242730CDB24}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E3B015B-6F91-49F2-A9A0-13B4642EEC29}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" activeTab="1" xr2:uid="{4F228711-34F2-CD4A-B88C-4A9EDC5CE2D1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4F228711-34F2-CD4A-B88C-4A9EDC5CE2D1}"/>
   </bookViews>
   <sheets>
     <sheet name="r0" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="152">
   <si>
     <t>Sample Flow Rate</t>
   </si>
@@ -477,6 +477,21 @@
   </si>
   <si>
     <t>Copy of 8v0 but change sample volume, sample flow rate, PBS wash post-sample flow rate</t>
+  </si>
+  <si>
+    <t>ExoT_r0_script_12v0</t>
+  </si>
+  <si>
+    <t>ExoT_r0_script_12v1</t>
+  </si>
+  <si>
+    <t>ExoT_r0_script_12v2</t>
+  </si>
+  <si>
+    <t>ExoT_r0_script_12v3</t>
+  </si>
+  <si>
+    <t>Andrew's flow rate optimization</t>
   </si>
 </sst>
 </file>
@@ -895,34 +910,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{865254A0-CD44-564E-904D-D988B38D1DFE}">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B16" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C30" sqref="C30"/>
+      <selection pane="bottomRight" activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.19921875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="49" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.69921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.19921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.69921875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.69921875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="20.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -957,7 +972,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -992,7 +1007,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>104</v>
       </c>
@@ -1027,7 +1042,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1062,7 +1077,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1097,7 +1112,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1132,7 +1147,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>65</v>
       </c>
@@ -1167,7 +1182,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>66</v>
       </c>
@@ -1202,7 +1217,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>67</v>
       </c>
@@ -1237,7 +1252,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -1272,7 +1287,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>69</v>
       </c>
@@ -1307,7 +1322,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>74</v>
       </c>
@@ -1342,7 +1357,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>77</v>
       </c>
@@ -1377,7 +1392,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>79</v>
       </c>
@@ -1412,7 +1427,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>80</v>
       </c>
@@ -1447,7 +1462,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>82</v>
       </c>
@@ -1479,7 +1494,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>83</v>
       </c>
@@ -1514,7 +1529,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>89</v>
       </c>
@@ -1549,7 +1564,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>90</v>
       </c>
@@ -1584,7 +1599,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>91</v>
       </c>
@@ -1619,7 +1634,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>92</v>
       </c>
@@ -1654,7 +1669,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>94</v>
       </c>
@@ -1689,7 +1704,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>95</v>
       </c>
@@ -1724,7 +1739,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>98</v>
       </c>
@@ -1759,7 +1774,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>100</v>
       </c>
@@ -1794,7 +1809,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>102</v>
       </c>
@@ -1829,7 +1844,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>108</v>
       </c>
@@ -1861,6 +1876,146 @@
         <v>23</v>
       </c>
       <c r="K29" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>147</v>
+      </c>
+      <c r="B30" t="s">
+        <v>151</v>
+      </c>
+      <c r="C30" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" t="s">
+        <v>30</v>
+      </c>
+      <c r="F30" t="s">
+        <v>76</v>
+      </c>
+      <c r="G30" t="s">
+        <v>87</v>
+      </c>
+      <c r="H30" t="s">
+        <v>14</v>
+      </c>
+      <c r="I30" t="s">
+        <v>28</v>
+      </c>
+      <c r="J30" t="s">
+        <v>23</v>
+      </c>
+      <c r="K30" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>148</v>
+      </c>
+      <c r="B31" t="s">
+        <v>151</v>
+      </c>
+      <c r="C31" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" t="s">
+        <v>30</v>
+      </c>
+      <c r="F31" t="s">
+        <v>76</v>
+      </c>
+      <c r="G31" t="s">
+        <v>71</v>
+      </c>
+      <c r="H31" t="s">
+        <v>14</v>
+      </c>
+      <c r="I31" t="s">
+        <v>28</v>
+      </c>
+      <c r="J31" t="s">
+        <v>23</v>
+      </c>
+      <c r="K31" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>149</v>
+      </c>
+      <c r="B32" t="s">
+        <v>151</v>
+      </c>
+      <c r="C32" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" t="s">
+        <v>30</v>
+      </c>
+      <c r="F32" t="s">
+        <v>76</v>
+      </c>
+      <c r="G32" t="s">
+        <v>15</v>
+      </c>
+      <c r="H32" t="s">
+        <v>14</v>
+      </c>
+      <c r="I32" t="s">
+        <v>28</v>
+      </c>
+      <c r="J32" t="s">
+        <v>23</v>
+      </c>
+      <c r="K32" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>150</v>
+      </c>
+      <c r="B33" t="s">
+        <v>151</v>
+      </c>
+      <c r="C33" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" t="s">
+        <v>30</v>
+      </c>
+      <c r="F33" t="s">
+        <v>76</v>
+      </c>
+      <c r="G33" t="s">
+        <v>72</v>
+      </c>
+      <c r="H33" t="s">
+        <v>14</v>
+      </c>
+      <c r="I33" t="s">
+        <v>28</v>
+      </c>
+      <c r="J33" t="s">
+        <v>23</v>
+      </c>
+      <c r="K33" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1874,25 +2029,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{789722DC-7BCB-4884-BC3A-D96FA1424135}">
   <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="M14" sqref="A14:M14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" customWidth="1"/>
-    <col min="2" max="2" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.796875" customWidth="1"/>
+    <col min="2" max="2" width="43.69921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.69921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.19921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.796875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.69921875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="25.5" customWidth="1"/>
-    <col min="11" max="11" width="20.6640625" customWidth="1"/>
-    <col min="12" max="12" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.69921875" customWidth="1"/>
+    <col min="12" max="12" width="20.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>85</v>
       </c>
@@ -1908,7 +2063,7 @@
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="3" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1950,7 +2105,7 @@
       </c>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>86</v>
       </c>
@@ -1986,7 +2141,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>110</v>
       </c>
@@ -2022,7 +2177,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>113</v>
       </c>
@@ -2061,7 +2216,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>116</v>
       </c>
@@ -2098,7 +2253,7 @@
       </c>
       <c r="M7" s="8"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>123</v>
       </c>
@@ -2139,7 +2294,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>125</v>
       </c>
@@ -2180,7 +2335,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>127</v>
       </c>
@@ -2221,7 +2376,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>132</v>
       </c>
@@ -2234,7 +2389,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>134</v>
       </c>
@@ -2242,7 +2397,7 @@
       <c r="H12" s="9"/>
       <c r="K12" s="8"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>137</v>
       </c>
@@ -2283,7 +2438,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>138</v>
       </c>
@@ -2324,19 +2479,19 @@
         <v>146</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="K15" s="8"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="K16" s="8"/>
     </row>
-    <row r="17" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K17" s="8"/>
     </row>
-    <row r="18" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K18" s="8"/>
     </row>
-    <row r="19" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="11:11" x14ac:dyDescent="0.3">
       <c r="K19" s="8"/>
     </row>
   </sheetData>
@@ -2352,14 +2507,14 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="50" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -2367,7 +2522,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -2375,10 +2530,10 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>41</v>
       </c>
@@ -2386,7 +2541,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>42</v>
       </c>
@@ -2394,10 +2549,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>36</v>
       </c>
@@ -2411,7 +2566,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2422,7 +2577,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2</v>
       </c>
@@ -2436,7 +2591,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>3</v>
       </c>
@@ -2450,7 +2605,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>4</v>
       </c>
@@ -2465,7 +2620,7 @@
       </c>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>5</v>
       </c>
@@ -2479,7 +2634,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>6</v>
       </c>
@@ -2493,7 +2648,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>7</v>
       </c>
@@ -2507,7 +2662,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>8</v>
       </c>
@@ -2521,7 +2676,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>9</v>
       </c>
@@ -2535,7 +2690,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>10</v>
       </c>
@@ -2549,7 +2704,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>11</v>
       </c>
@@ -2563,7 +2718,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Added 7v3 and 10v0
To discuss before creating updated T2 protocol
</commit_message>
<xml_diff>
--- a/r0 SCRIPTS.xlsx
+++ b/r0 SCRIPTS.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josh.buser\Documents\GitHub\cd-alpha\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chipdx/Documents/Protocols/r0 and v0 SCRIPT PROTOCOLS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E3B015B-6F91-49F2-A9A0-13B4642EEC29}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CF8117C-0AB6-BC4C-9936-ABA6BD63B738}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4F228711-34F2-CD4A-B88C-4A9EDC5CE2D1}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" activeTab="1" xr2:uid="{4F228711-34F2-CD4A-B88C-4A9EDC5CE2D1}"/>
   </bookViews>
   <sheets>
     <sheet name="r0" sheetId="1" r:id="rId1"/>
     <sheet name="v0" sheetId="3" r:id="rId2"/>
     <sheet name="1v0" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterateCount="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="159">
   <si>
     <t>Sample Flow Rate</t>
   </si>
@@ -492,6 +492,27 @@
   </si>
   <si>
     <t>Andrew's flow rate optimization</t>
+  </si>
+  <si>
+    <t>v0-protocol-10v0.json</t>
+  </si>
+  <si>
+    <t>T2 - 0.5 mL MNP 'sample'</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Updating 7v2 with new protocol changes and sending initial pull to waste instead of lysate syringe to decrease sample dilution</t>
+  </si>
+  <si>
+    <t>v0-protocol-7v3.json</t>
+  </si>
+  <si>
+    <t>Update 7v2: 1.4 mL F-127 (pull 1 mL); pull 1.05 mL PBS (after F-127)</t>
+  </si>
+  <si>
+    <t>500 (PBS chase)</t>
   </si>
 </sst>
 </file>
@@ -576,7 +597,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -595,6 +616,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -912,32 +936,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{865254A0-CD44-564E-904D-D988B38D1DFE}">
   <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
       <selection pane="bottomRight" activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="49" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.19921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.69921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.19921875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.69921875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.69921875" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="20.296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -972,7 +996,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1007,7 +1031,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>104</v>
       </c>
@@ -1042,7 +1066,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1077,7 +1101,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1112,7 +1136,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1147,7 +1171,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>65</v>
       </c>
@@ -1182,7 +1206,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>66</v>
       </c>
@@ -1217,7 +1241,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>67</v>
       </c>
@@ -1252,7 +1276,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -1287,7 +1311,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>69</v>
       </c>
@@ -1322,7 +1346,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>74</v>
       </c>
@@ -1357,7 +1381,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>77</v>
       </c>
@@ -1392,7 +1416,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>79</v>
       </c>
@@ -1427,7 +1451,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>80</v>
       </c>
@@ -1462,7 +1486,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>82</v>
       </c>
@@ -1494,7 +1518,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>83</v>
       </c>
@@ -1529,7 +1553,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>89</v>
       </c>
@@ -1564,7 +1588,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>90</v>
       </c>
@@ -1599,7 +1623,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>91</v>
       </c>
@@ -1634,7 +1658,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>92</v>
       </c>
@@ -1669,7 +1693,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>94</v>
       </c>
@@ -1704,7 +1728,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>95</v>
       </c>
@@ -1739,7 +1763,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>98</v>
       </c>
@@ -1774,7 +1798,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>100</v>
       </c>
@@ -1809,7 +1833,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>102</v>
       </c>
@@ -1844,7 +1868,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>108</v>
       </c>
@@ -1879,7 +1903,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>147</v>
       </c>
@@ -1914,7 +1938,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>148</v>
       </c>
@@ -1949,7 +1973,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>149</v>
       </c>
@@ -1984,7 +2008,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>150</v>
       </c>
@@ -2027,27 +2051,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{789722DC-7BCB-4884-BC3A-D96FA1424135}">
-  <dimension ref="A1:O19"/>
+  <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="M14" sqref="A14:M14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.796875" customWidth="1"/>
-    <col min="2" max="2" width="43.69921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.69921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.19921875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.83203125" customWidth="1"/>
+    <col min="2" max="2" width="43.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.69921875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="25.5" customWidth="1"/>
-    <col min="11" max="11" width="20.69921875" customWidth="1"/>
-    <col min="12" max="12" width="20.296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.6640625" customWidth="1"/>
+    <col min="12" max="12" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>85</v>
       </c>
@@ -2063,7 +2087,7 @@
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="3" spans="1:15" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2105,7 +2129,7 @@
       </c>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>86</v>
       </c>
@@ -2133,7 +2157,7 @@
       <c r="I4" t="s">
         <v>28</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="8" t="s">
         <v>23</v>
       </c>
       <c r="K4" s="8"/>
@@ -2141,7 +2165,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>110</v>
       </c>
@@ -2169,7 +2193,7 @@
       <c r="I5" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="8" t="s">
         <v>114</v>
       </c>
       <c r="K5" s="8"/>
@@ -2177,7 +2201,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>113</v>
       </c>
@@ -2205,7 +2229,7 @@
       <c r="I6" t="s">
         <v>28</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="8" t="s">
         <v>114</v>
       </c>
       <c r="K6" s="8"/>
@@ -2216,7 +2240,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>116</v>
       </c>
@@ -2244,7 +2268,7 @@
       <c r="I7">
         <v>500</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="8" t="s">
         <v>118</v>
       </c>
       <c r="K7" s="8"/>
@@ -2253,7 +2277,7 @@
       </c>
       <c r="M7" s="8"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>123</v>
       </c>
@@ -2281,7 +2305,7 @@
       <c r="I8" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="J8" s="8" t="s">
         <v>121</v>
       </c>
       <c r="K8" s="11" t="s">
@@ -2294,7 +2318,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>125</v>
       </c>
@@ -2322,7 +2346,7 @@
       <c r="I9" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="J9" s="8" t="s">
         <v>121</v>
       </c>
       <c r="K9" s="11" t="s">
@@ -2335,7 +2359,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>127</v>
       </c>
@@ -2363,7 +2387,7 @@
       <c r="I10" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="J10" s="5" t="s">
+      <c r="J10" s="8" t="s">
         <v>121</v>
       </c>
       <c r="K10" s="11" t="s">
@@ -2376,12 +2400,13 @@
         <v>130</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>132</v>
       </c>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
+      <c r="J11" s="8"/>
       <c r="K11" s="11" t="s">
         <v>142</v>
       </c>
@@ -2389,84 +2414,56 @@
         <v>133</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>134</v>
       </c>
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
+      <c r="J12" s="8"/>
       <c r="K12" s="8"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>156</v>
+      </c>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="M13" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>137</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>136</v>
       </c>
-      <c r="C13" t="s">
-        <v>12</v>
-      </c>
-      <c r="D13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" t="s">
-        <v>30</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="C14" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" t="s">
         <v>120</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G14" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="H13" s="9" t="s">
+      <c r="H14" s="9" t="s">
         <v>71</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="K13" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="L13" t="s">
-        <v>25</v>
-      </c>
-      <c r="M13" s="8" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>138</v>
-      </c>
-      <c r="B14" t="s">
-        <v>139</v>
-      </c>
-      <c r="C14" t="s">
-        <v>12</v>
-      </c>
-      <c r="D14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" t="s">
-        <v>30</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>14</v>
       </c>
       <c r="I14" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="J14" s="5" t="s">
+      <c r="J14" s="8" t="s">
         <v>121</v>
       </c>
       <c r="K14" s="11" t="s">
@@ -2476,23 +2473,104 @@
         <v>25</v>
       </c>
       <c r="M14" s="8" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>138</v>
+      </c>
+      <c r="B15" t="s">
+        <v>139</v>
+      </c>
+      <c r="C15" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="K15" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="L15" t="s">
+        <v>25</v>
+      </c>
+      <c r="M15" s="8" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="K15" s="8"/>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="K16" s="8"/>
-    </row>
-    <row r="17" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>152</v>
+      </c>
+      <c r="B16" t="s">
+        <v>153</v>
+      </c>
+      <c r="C16" t="s">
+        <v>12</v>
+      </c>
+      <c r="D16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="J16" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="K16" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="L16" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="M16" s="11" t="s">
+        <v>155</v>
+      </c>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+    </row>
+    <row r="17" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K17" s="8"/>
     </row>
-    <row r="18" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K18" s="8"/>
     </row>
-    <row r="19" spans="11:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="11:11" x14ac:dyDescent="0.2">
       <c r="K19" s="8"/>
+    </row>
+    <row r="20" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K20" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2507,14 +2585,14 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="50" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -2522,7 +2600,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -2530,10 +2608,10 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>41</v>
       </c>
@@ -2541,7 +2619,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>42</v>
       </c>
@@ -2549,10 +2627,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>36</v>
       </c>
@@ -2566,7 +2644,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2577,7 +2655,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2</v>
       </c>
@@ -2591,7 +2669,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>3</v>
       </c>
@@ -2605,7 +2683,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>4</v>
       </c>
@@ -2620,7 +2698,7 @@
       </c>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>5</v>
       </c>
@@ -2634,7 +2712,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>6</v>
       </c>
@@ -2648,7 +2726,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>7</v>
       </c>
@@ -2662,7 +2740,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>8</v>
       </c>
@@ -2676,7 +2754,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>9</v>
       </c>
@@ -2690,7 +2768,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>10</v>
       </c>
@@ -2704,7 +2782,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>11</v>
       </c>
@@ -2718,7 +2796,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Added v0 11v0 and 12v0
T2 no PBS chase 1 and 10 mL/hr scripts
</commit_message>
<xml_diff>
--- a/r0 SCRIPTS.xlsx
+++ b/r0 SCRIPTS.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chipdx/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chipdx/Documents/Protocols/r0 and v0 SCRIPT PROTOCOLS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21A11F64-C38A-544D-919D-43CEAB37DA55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{944C61FF-4533-B34A-8F30-C3634D55FEC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15300" activeTab="1" xr2:uid="{4F228711-34F2-CD4A-B88C-4A9EDC5CE2D1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="169">
   <si>
     <t>Sample Flow Rate</t>
   </si>
@@ -516,13 +516,40 @@
   </si>
   <si>
     <t>Y - 1 mL, pull 0.8 mL to lysate @ 25 mL/hr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T2 (PBS Chase) </t>
+  </si>
+  <si>
+    <t>v0-protocol-11v0.json</t>
+  </si>
+  <si>
+    <t>1 mL/hr</t>
+  </si>
+  <si>
+    <t>v0-protocol-12v0.json</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Exact copy of 11v0 except 10 mL/hr instead of 1 mL/hr</t>
+  </si>
+  <si>
+    <t>Can use 7v3 as reference - remove extra 2 min incubation after F-127; change sample flow rate to 1 mL/hr; sample pull 500 ul to waste syringe then 1 mL to lysate/collection syringe</t>
+  </si>
+  <si>
+    <t>T2 (No PBS Chase) 1 mL/hr</t>
+  </si>
+  <si>
+    <t>T2 (No PBS Chase) 10 mL/hr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -573,6 +600,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -600,7 +635,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -620,6 +655,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2053,8 +2089,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{789722DC-7BCB-4884-BC3A-D96FA1424135}">
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2427,6 +2463,9 @@
       <c r="A13" t="s">
         <v>153</v>
       </c>
+      <c r="B13" t="s">
+        <v>160</v>
+      </c>
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
       <c r="J13" s="8"/>
@@ -2555,16 +2594,92 @@
         <v>159</v>
       </c>
     </row>
-    <row r="17" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K17" s="8"/>
-    </row>
-    <row r="18" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K18" s="8"/>
-    </row>
-    <row r="19" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>161</v>
+      </c>
+      <c r="B17" t="s">
+        <v>167</v>
+      </c>
+      <c r="C17" t="s">
+        <v>12</v>
+      </c>
+      <c r="D17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" t="s">
+        <v>106</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="H17" t="s">
+        <v>164</v>
+      </c>
+      <c r="I17" t="s">
+        <v>164</v>
+      </c>
+      <c r="J17" t="s">
+        <v>164</v>
+      </c>
+      <c r="K17" t="s">
+        <v>164</v>
+      </c>
+      <c r="L17" t="s">
+        <v>164</v>
+      </c>
+      <c r="M17" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>163</v>
+      </c>
+      <c r="B18" t="s">
+        <v>168</v>
+      </c>
+      <c r="C18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" t="s">
+        <v>106</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="H18" t="s">
+        <v>164</v>
+      </c>
+      <c r="I18" t="s">
+        <v>164</v>
+      </c>
+      <c r="J18" t="s">
+        <v>164</v>
+      </c>
+      <c r="K18" t="s">
+        <v>164</v>
+      </c>
+      <c r="L18" t="s">
+        <v>164</v>
+      </c>
+      <c r="M18" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="K19" s="8"/>
     </row>
-    <row r="20" spans="11:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="K20" s="8"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added v0 scripts 14v0, 15v0, 16v0
T2 and western v0 scripts
</commit_message>
<xml_diff>
--- a/r0 SCRIPTS.xlsx
+++ b/r0 SCRIPTS.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chipdx/Documents/Protocols/r0 and v0 SCRIPT PROTOCOLS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chipdx/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80481C75-9E31-334B-B2D8-CDBFA899D9D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBEE5F6-B952-A94F-B8A9-0FF9C5243995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15300" activeTab="1" xr2:uid="{4F228711-34F2-CD4A-B88C-4A9EDC5CE2D1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="183">
   <si>
     <t>Sample Flow Rate</t>
   </si>
@@ -552,6 +552,39 @@
   </si>
   <si>
     <t>See QC Checklist_v0-protocol-13v0.xlsx and ChipDx Fluid Flow Visual Model_13v0_071921.pptx (concentrated sample, pull reservoir to 0, 200-800-1000 PBS chase structure)</t>
+  </si>
+  <si>
+    <t>v0-protocol-14v0.json</t>
+  </si>
+  <si>
+    <t>v0-protocol-15v0.json</t>
+  </si>
+  <si>
+    <t>T2 5 mL/hr (concentrated sample, PBS chases)</t>
+  </si>
+  <si>
+    <t>T2 1 mL/hr (concentrated sample, PBS chases)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exact copy of 13v0 except 5 mL/hr instead of 10 mL/hr for sample and PBS washes </t>
+  </si>
+  <si>
+    <t>1 mL/hr (200) then 5 mL/hr (800, 1000)</t>
+  </si>
+  <si>
+    <t>Exact copy of 13v0 except 1 mL/hr instead of 10 mL/hr for sample and 200 uL PBS wash, 5 mL/hr for 800 and 1000 PBS wash</t>
+  </si>
+  <si>
+    <t>v0-protocol-16v0.json</t>
+  </si>
+  <si>
+    <t>Western Blot 2</t>
+  </si>
+  <si>
+    <t>waste/500 + lysate/200 @ 50 mL/hr</t>
+  </si>
+  <si>
+    <t>Pull sample, last PBS wash, and QIAzol down to 0 mL to decrease sample dilution</t>
   </si>
 </sst>
 </file>
@@ -982,10 +1015,10 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A30" sqref="A30"/>
+      <selection pane="bottomRight" activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2096,10 +2129,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{789722DC-7BCB-4884-BC3A-D96FA1424135}">
-  <dimension ref="A1:O20"/>
+  <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2109,7 +2142,7 @@
     <col min="3" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="25.5" customWidth="1"/>
     <col min="11" max="11" width="31.5" bestFit="1" customWidth="1"/>
@@ -2727,7 +2760,127 @@
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="K20" s="8"/>
+      <c r="A20" t="s">
+        <v>172</v>
+      </c>
+      <c r="B20" t="s">
+        <v>174</v>
+      </c>
+      <c r="C20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" t="s">
+        <v>106</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="H20" t="s">
+        <v>71</v>
+      </c>
+      <c r="I20" t="s">
+        <v>28</v>
+      </c>
+      <c r="J20" t="s">
+        <v>164</v>
+      </c>
+      <c r="K20" t="s">
+        <v>164</v>
+      </c>
+      <c r="L20" t="s">
+        <v>164</v>
+      </c>
+      <c r="M20" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>173</v>
+      </c>
+      <c r="B21" t="s">
+        <v>175</v>
+      </c>
+      <c r="C21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" t="s">
+        <v>106</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="H21" t="s">
+        <v>177</v>
+      </c>
+      <c r="I21" t="s">
+        <v>28</v>
+      </c>
+      <c r="J21" t="s">
+        <v>164</v>
+      </c>
+      <c r="K21" t="s">
+        <v>164</v>
+      </c>
+      <c r="L21" t="s">
+        <v>164</v>
+      </c>
+      <c r="M21" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>179</v>
+      </c>
+      <c r="B22" t="s">
+        <v>180</v>
+      </c>
+      <c r="C22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" t="s">
+        <v>30</v>
+      </c>
+      <c r="F22" t="s">
+        <v>76</v>
+      </c>
+      <c r="G22" t="s">
+        <v>15</v>
+      </c>
+      <c r="H22" t="s">
+        <v>15</v>
+      </c>
+      <c r="I22" t="s">
+        <v>28</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="K22" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="L22" t="s">
+        <v>159</v>
+      </c>
+      <c r="M22" s="8" t="s">
+        <v>182</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update 14v0 and 15v0
</commit_message>
<xml_diff>
--- a/r0 SCRIPTS.xlsx
+++ b/r0 SCRIPTS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chipdx/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBEE5F6-B952-A94F-B8A9-0FF9C5243995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E93CF66D-494A-C045-AACC-03F648F9B572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15300" activeTab="1" xr2:uid="{4F228711-34F2-CD4A-B88C-4A9EDC5CE2D1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="184">
   <si>
     <t>Sample Flow Rate</t>
   </si>
@@ -566,15 +566,6 @@
     <t>T2 1 mL/hr (concentrated sample, PBS chases)</t>
   </si>
   <si>
-    <t xml:space="preserve">Exact copy of 13v0 except 5 mL/hr instead of 10 mL/hr for sample and PBS washes </t>
-  </si>
-  <si>
-    <t>1 mL/hr (200) then 5 mL/hr (800, 1000)</t>
-  </si>
-  <si>
-    <t>Exact copy of 13v0 except 1 mL/hr instead of 10 mL/hr for sample and 200 uL PBS wash, 5 mL/hr for 800 and 1000 PBS wash</t>
-  </si>
-  <si>
     <t>v0-protocol-16v0.json</t>
   </si>
   <si>
@@ -585,6 +576,18 @@
   </si>
   <si>
     <t>Pull sample, last PBS wash, and QIAzol down to 0 mL to decrease sample dilution</t>
+  </si>
+  <si>
+    <t>5 mL/hr (200 + 400/800) then 10 mL/hr (400/800 + 1000)</t>
+  </si>
+  <si>
+    <t>1 mL/hr (200 + 400/800) then 10 mL/hr (400/800 + 1000)</t>
+  </si>
+  <si>
+    <t>Exact copy of 13v0 except 5 mL/hr flow rate, update flow rate PBS washes</t>
+  </si>
+  <si>
+    <t>Exact copy of 14v0 except 1 mL/hr flow rate, update flow rate PBS washes</t>
   </si>
 </sst>
 </file>
@@ -2131,8 +2134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{789722DC-7BCB-4884-BC3A-D96FA1424135}">
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2782,7 +2785,7 @@
         <v>71</v>
       </c>
       <c r="H20" t="s">
-        <v>71</v>
+        <v>180</v>
       </c>
       <c r="I20" t="s">
         <v>28</v>
@@ -2797,7 +2800,7 @@
         <v>164</v>
       </c>
       <c r="M20" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
@@ -2823,7 +2826,7 @@
         <v>162</v>
       </c>
       <c r="H21" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="I21" t="s">
         <v>28</v>
@@ -2838,15 +2841,15 @@
         <v>164</v>
       </c>
       <c r="M21" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B22" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C22" t="s">
         <v>12</v>
@@ -2873,13 +2876,13 @@
         <v>114</v>
       </c>
       <c r="K22" s="8" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="L22" t="s">
         <v>159</v>
       </c>
       <c r="M22" s="8" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add 13v0 r0 for griffin
</commit_message>
<xml_diff>
--- a/r0 SCRIPTS.xlsx
+++ b/r0 SCRIPTS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chipdx/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josh.buser\OneDrive - chip-diagnostics.com\Documents\GitHub\cd-alpha\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E93CF66D-494A-C045-AACC-03F648F9B572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18E40974-1386-404E-B26D-A80441C3333A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15300" activeTab="1" xr2:uid="{4F228711-34F2-CD4A-B88C-4A9EDC5CE2D1}"/>
+    <workbookView xWindow="1884" yWindow="1884" windowWidth="9528" windowHeight="8484" xr2:uid="{4F228711-34F2-CD4A-B88C-4A9EDC5CE2D1}"/>
   </bookViews>
   <sheets>
     <sheet name="r0" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="186">
   <si>
     <t>Sample Flow Rate</t>
   </si>
@@ -588,6 +588,12 @@
   </si>
   <si>
     <t>Exact copy of 14v0 except 1 mL/hr flow rate, update flow rate PBS washes</t>
+  </si>
+  <si>
+    <t>ExoT_r0_script_13v0</t>
+  </si>
+  <si>
+    <t>Griffin qiazol elution</t>
   </si>
 </sst>
 </file>
@@ -1015,34 +1021,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{865254A0-CD44-564E-904D-D988B38D1DFE}">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:K34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="I31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B33" sqref="B33"/>
+      <selection pane="bottomRight" activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.19921875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="49" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.69921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.19921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.69921875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.69921875" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="20.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1077,7 +1083,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1112,7 +1118,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>104</v>
       </c>
@@ -1147,7 +1153,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1182,7 +1188,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1217,7 +1223,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1252,7 +1258,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>65</v>
       </c>
@@ -1287,7 +1293,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>66</v>
       </c>
@@ -1322,7 +1328,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>67</v>
       </c>
@@ -1357,7 +1363,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -1392,7 +1398,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>69</v>
       </c>
@@ -1427,7 +1433,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>74</v>
       </c>
@@ -1462,7 +1468,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>77</v>
       </c>
@@ -1497,7 +1503,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>79</v>
       </c>
@@ -1532,7 +1538,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>80</v>
       </c>
@@ -1567,7 +1573,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>82</v>
       </c>
@@ -1599,7 +1605,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>83</v>
       </c>
@@ -1634,7 +1640,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>89</v>
       </c>
@@ -1669,7 +1675,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>90</v>
       </c>
@@ -1704,7 +1710,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>91</v>
       </c>
@@ -1739,7 +1745,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>92</v>
       </c>
@@ -1774,7 +1780,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>94</v>
       </c>
@@ -1809,7 +1815,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>95</v>
       </c>
@@ -1844,7 +1850,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>98</v>
       </c>
@@ -1879,7 +1885,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>100</v>
       </c>
@@ -1914,7 +1920,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>102</v>
       </c>
@@ -1949,7 +1955,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>108</v>
       </c>
@@ -1984,7 +1990,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>147</v>
       </c>
@@ -2019,7 +2025,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>148</v>
       </c>
@@ -2054,7 +2060,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>149</v>
       </c>
@@ -2089,7 +2095,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>150</v>
       </c>
@@ -2121,6 +2127,41 @@
         <v>23</v>
       </c>
       <c r="K33" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>184</v>
+      </c>
+      <c r="B34" t="s">
+        <v>185</v>
+      </c>
+      <c r="C34" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" t="s">
+        <v>30</v>
+      </c>
+      <c r="F34" t="s">
+        <v>20</v>
+      </c>
+      <c r="G34" t="s">
+        <v>14</v>
+      </c>
+      <c r="H34" t="s">
+        <v>14</v>
+      </c>
+      <c r="I34" t="s">
+        <v>28</v>
+      </c>
+      <c r="J34" t="s">
+        <v>23</v>
+      </c>
+      <c r="K34" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2134,25 +2175,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{789722DC-7BCB-4884-BC3A-D96FA1424135}">
   <dimension ref="A1:O22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="D4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" customWidth="1"/>
-    <col min="2" max="2" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="34.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.796875" customWidth="1"/>
+    <col min="2" max="2" width="43.69921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.69921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.19921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.19921875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.69921875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="25.5" customWidth="1"/>
     <col min="11" max="11" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="36.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>85</v>
       </c>
@@ -2168,7 +2209,7 @@
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="3" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="46.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2210,7 +2251,7 @@
       </c>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>86</v>
       </c>
@@ -2246,7 +2287,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>110</v>
       </c>
@@ -2282,7 +2323,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>113</v>
       </c>
@@ -2321,7 +2362,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>116</v>
       </c>
@@ -2358,7 +2399,7 @@
       </c>
       <c r="M7" s="8"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>123</v>
       </c>
@@ -2399,7 +2440,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>125</v>
       </c>
@@ -2440,7 +2481,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>127</v>
       </c>
@@ -2481,7 +2522,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>132</v>
       </c>
@@ -2495,7 +2536,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>134</v>
       </c>
@@ -2504,7 +2545,7 @@
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>153</v>
       </c>
@@ -2519,7 +2560,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>137</v>
       </c>
@@ -2560,7 +2601,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>138</v>
       </c>
@@ -2601,7 +2642,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>152</v>
       </c>
@@ -2639,7 +2680,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>161</v>
       </c>
@@ -2680,7 +2721,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>163</v>
       </c>
@@ -2721,7 +2762,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>169</v>
       </c>
@@ -2762,7 +2803,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>172</v>
       </c>
@@ -2803,7 +2844,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>173</v>
       </c>
@@ -2844,7 +2885,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>176</v>
       </c>
@@ -2898,14 +2939,14 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.296875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="50" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -2913,7 +2954,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -2921,10 +2962,10 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>41</v>
       </c>
@@ -2932,7 +2973,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>42</v>
       </c>
@@ -2940,10 +2981,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>36</v>
       </c>
@@ -2957,7 +2998,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2968,7 +3009,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>2</v>
       </c>
@@ -2982,7 +3023,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>3</v>
       </c>
@@ -2996,7 +3037,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>4</v>
       </c>
@@ -3011,7 +3052,7 @@
       </c>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>5</v>
       </c>
@@ -3025,7 +3066,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>6</v>
       </c>
@@ -3039,7 +3080,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>7</v>
       </c>
@@ -3053,7 +3094,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>8</v>
       </c>
@@ -3067,7 +3108,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>9</v>
       </c>
@@ -3081,7 +3122,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>10</v>
       </c>
@@ -3095,7 +3136,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>11</v>
       </c>
@@ -3109,7 +3150,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Add 14v0 r0 script for Issadore lab
</commit_message>
<xml_diff>
--- a/r0 SCRIPTS.xlsx
+++ b/r0 SCRIPTS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chipdx/Documents/Protocols/r0 and v0 SCRIPT PROTOCOLS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://netorg4197135-my.sharepoint.com/personal/will_brown_chip-diagnostics_com/Documents/Documents/Github/cd-alpha/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56D8781F-64E5-0E4B-96A7-1774F22AB709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{56D8781F-64E5-0E4B-96A7-1774F22AB709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8ED1ED5-020A-4065-AB13-CEE09EEC7460}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" activeTab="1" xr2:uid="{4F228711-34F2-CD4A-B88C-4A9EDC5CE2D1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4F228711-34F2-CD4A-B88C-4A9EDC5CE2D1}"/>
   </bookViews>
   <sheets>
     <sheet name="r0" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="205">
   <si>
     <t>Sample Flow Rate</t>
   </si>
@@ -639,6 +639,18 @@
   </si>
   <si>
     <t xml:space="preserve">Modification of 16v2 - change RIPA to QIAzol, add 700 uL QIAzol and pull 600 uL to waste then 100 uL to lysate; final PBS chase pull 0.8 mL AND 0.2 mL less on first PBS rinse to keep total waste syringe vol &lt;6 mL </t>
+  </si>
+  <si>
+    <t>ExoT_r0_script_14v0</t>
+  </si>
+  <si>
+    <t>Issadore Alzheimer's DLB Project</t>
+  </si>
+  <si>
+    <t>700-700-700</t>
+  </si>
+  <si>
+    <t>0 mins</t>
   </si>
 </sst>
 </file>
@@ -731,7 +743,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -742,12 +754,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1066,34 +1072,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{865254A0-CD44-564E-904D-D988B38D1DFE}">
-  <dimension ref="A1:K34"/>
+  <dimension ref="A1:K35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="K8" sqref="K8"/>
+      <selection pane="bottomRight" activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="49" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="20.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1128,7 +1134,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1163,7 +1169,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>104</v>
       </c>
@@ -1198,7 +1204,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1233,7 +1239,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1268,7 +1274,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1303,7 +1309,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>65</v>
       </c>
@@ -1338,7 +1344,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>66</v>
       </c>
@@ -1373,7 +1379,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>67</v>
       </c>
@@ -1408,7 +1414,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -1443,7 +1449,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>69</v>
       </c>
@@ -1478,7 +1484,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>74</v>
       </c>
@@ -1513,7 +1519,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>77</v>
       </c>
@@ -1548,7 +1554,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>79</v>
       </c>
@@ -1583,7 +1589,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>80</v>
       </c>
@@ -1618,7 +1624,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>82</v>
       </c>
@@ -1650,7 +1656,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>83</v>
       </c>
@@ -1685,7 +1691,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>89</v>
       </c>
@@ -1720,7 +1726,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>90</v>
       </c>
@@ -1755,7 +1761,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>91</v>
       </c>
@@ -1790,7 +1796,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>92</v>
       </c>
@@ -1825,7 +1831,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>94</v>
       </c>
@@ -1860,7 +1866,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>95</v>
       </c>
@@ -1895,7 +1901,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>98</v>
       </c>
@@ -1930,7 +1936,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>100</v>
       </c>
@@ -1965,7 +1971,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>102</v>
       </c>
@@ -2000,7 +2006,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>108</v>
       </c>
@@ -2035,7 +2041,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>147</v>
       </c>
@@ -2070,7 +2076,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>148</v>
       </c>
@@ -2105,7 +2111,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>149</v>
       </c>
@@ -2140,7 +2146,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>150</v>
       </c>
@@ -2175,7 +2181,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>184</v>
       </c>
@@ -2207,6 +2213,41 @@
         <v>23</v>
       </c>
       <c r="K34" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>201</v>
+      </c>
+      <c r="B35" t="s">
+        <v>202</v>
+      </c>
+      <c r="C35" t="s">
+        <v>12</v>
+      </c>
+      <c r="D35" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" t="s">
+        <v>30</v>
+      </c>
+      <c r="F35" t="s">
+        <v>18</v>
+      </c>
+      <c r="G35" t="s">
+        <v>162</v>
+      </c>
+      <c r="H35" t="s">
+        <v>14</v>
+      </c>
+      <c r="I35" t="s">
+        <v>203</v>
+      </c>
+      <c r="J35" t="s">
+        <v>204</v>
+      </c>
+      <c r="K35" t="s">
         <v>25</v>
       </c>
     </row>
@@ -2220,25 +2261,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{789722DC-7BCB-4884-BC3A-D96FA1424135}">
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.83203125" customWidth="1"/>
-    <col min="2" max="2" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="34.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.875" customWidth="1"/>
+    <col min="2" max="2" width="43.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="25.5" customWidth="1"/>
     <col min="11" max="11" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="36.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>85</v>
       </c>
@@ -2254,7 +2295,7 @@
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="3" spans="1:15" ht="34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2282,10 +2323,10 @@
       <c r="I3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="8" t="s">
         <v>144</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="K3" s="8" t="s">
         <v>143</v>
       </c>
       <c r="L3" s="1" t="s">
@@ -2296,7 +2337,7 @@
       </c>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>86</v>
       </c>
@@ -2324,15 +2365,14 @@
       <c r="I4" t="s">
         <v>28</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="J4" t="s">
         <v>23</v>
       </c>
-      <c r="K4" s="8"/>
       <c r="L4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>110</v>
       </c>
@@ -2360,15 +2400,14 @@
       <c r="I5" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="J5" t="s">
         <v>114</v>
       </c>
-      <c r="K5" s="8"/>
       <c r="L5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>113</v>
       </c>
@@ -2396,18 +2435,17 @@
       <c r="I6" t="s">
         <v>28</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="J6" t="s">
         <v>114</v>
       </c>
-      <c r="K6" s="8"/>
       <c r="L6" t="s">
         <v>25</v>
       </c>
-      <c r="M6" s="8" t="s">
+      <c r="M6" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>116</v>
       </c>
@@ -2426,25 +2464,23 @@
       <c r="F7" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H7" s="9" t="s">
+      <c r="G7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" t="s">
         <v>14</v>
       </c>
       <c r="I7">
         <v>500</v>
       </c>
-      <c r="J7" s="8" t="s">
+      <c r="J7" t="s">
         <v>118</v>
       </c>
-      <c r="K7" s="8"/>
       <c r="L7" t="s">
         <v>25</v>
       </c>
-      <c r="M7" s="8"/>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>123</v>
       </c>
@@ -2463,29 +2499,29 @@
       <c r="F8" t="s">
         <v>120</v>
       </c>
-      <c r="G8" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" s="9" t="s">
+      <c r="G8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H8" t="s">
         <v>14</v>
       </c>
       <c r="I8" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="J8" s="8" t="s">
+      <c r="J8" t="s">
         <v>121</v>
       </c>
-      <c r="K8" s="11" t="s">
+      <c r="K8" t="s">
         <v>140</v>
       </c>
       <c r="L8" t="s">
         <v>25</v>
       </c>
-      <c r="M8" s="8" t="s">
+      <c r="M8" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>125</v>
       </c>
@@ -2504,29 +2540,29 @@
       <c r="F9" t="s">
         <v>120</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" t="s">
         <v>129</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="H9" t="s">
         <v>71</v>
       </c>
       <c r="I9" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="J9" s="8" t="s">
+      <c r="J9" t="s">
         <v>121</v>
       </c>
-      <c r="K9" s="11" t="s">
+      <c r="K9" t="s">
         <v>140</v>
       </c>
       <c r="L9" t="s">
         <v>25</v>
       </c>
-      <c r="M9" s="8" t="s">
+      <c r="M9" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>127</v>
       </c>
@@ -2545,19 +2581,19 @@
       <c r="F10" t="s">
         <v>18</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G10" t="s">
         <v>129</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="H10" t="s">
         <v>71</v>
       </c>
       <c r="I10" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="J10" s="8" t="s">
+      <c r="J10" t="s">
         <v>121</v>
       </c>
-      <c r="K10" s="11" t="s">
+      <c r="K10" t="s">
         <v>141</v>
       </c>
       <c r="L10" t="s">
@@ -2567,45 +2603,34 @@
         <v>130</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>132</v>
       </c>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="11" t="s">
+      <c r="K11" t="s">
         <v>142</v>
       </c>
       <c r="M11" s="5" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>134</v>
       </c>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>153</v>
       </c>
       <c r="B13" t="s">
         <v>160</v>
       </c>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
       <c r="M13" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>137</v>
       </c>
@@ -2624,29 +2649,29 @@
       <c r="F14" t="s">
         <v>120</v>
       </c>
-      <c r="G14" s="9" t="s">
+      <c r="G14" t="s">
         <v>87</v>
       </c>
-      <c r="H14" s="9" t="s">
+      <c r="H14" t="s">
         <v>71</v>
       </c>
       <c r="I14" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="J14" s="8" t="s">
+      <c r="J14" t="s">
         <v>121</v>
       </c>
-      <c r="K14" s="11" t="s">
+      <c r="K14" t="s">
         <v>142</v>
       </c>
       <c r="L14" t="s">
         <v>25</v>
       </c>
-      <c r="M14" s="8" t="s">
+      <c r="M14" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>138</v>
       </c>
@@ -2674,20 +2699,20 @@
       <c r="I15" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="J15" s="8" t="s">
+      <c r="J15" t="s">
         <v>121</v>
       </c>
-      <c r="K15" s="11" t="s">
+      <c r="K15" t="s">
         <v>142</v>
       </c>
       <c r="L15" t="s">
         <v>25</v>
       </c>
-      <c r="M15" s="8" t="s">
+      <c r="M15" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>152</v>
       </c>
@@ -2725,7 +2750,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>161</v>
       </c>
@@ -2744,7 +2769,7 @@
       <c r="F17" t="s">
         <v>106</v>
       </c>
-      <c r="G17" s="13" t="s">
+      <c r="G17" s="9" t="s">
         <v>162</v>
       </c>
       <c r="H17" t="s">
@@ -2766,7 +2791,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>163</v>
       </c>
@@ -2785,7 +2810,7 @@
       <c r="F18" t="s">
         <v>106</v>
       </c>
-      <c r="G18" s="13" t="s">
+      <c r="G18" s="9" t="s">
         <v>15</v>
       </c>
       <c r="H18" t="s">
@@ -2807,7 +2832,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>169</v>
       </c>
@@ -2826,7 +2851,7 @@
       <c r="F19" t="s">
         <v>106</v>
       </c>
-      <c r="G19" s="9" t="s">
+      <c r="G19" t="s">
         <v>15</v>
       </c>
       <c r="H19" t="s">
@@ -2848,7 +2873,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>172</v>
       </c>
@@ -2867,7 +2892,7 @@
       <c r="F20" t="s">
         <v>106</v>
       </c>
-      <c r="G20" s="9" t="s">
+      <c r="G20" t="s">
         <v>71</v>
       </c>
       <c r="H20" t="s">
@@ -2889,7 +2914,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>173</v>
       </c>
@@ -2908,7 +2933,7 @@
       <c r="F21" t="s">
         <v>106</v>
       </c>
-      <c r="G21" s="9" t="s">
+      <c r="G21" t="s">
         <v>162</v>
       </c>
       <c r="H21" t="s">
@@ -2930,7 +2955,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>176</v>
       </c>
@@ -2958,20 +2983,20 @@
       <c r="I22" t="s">
         <v>28</v>
       </c>
-      <c r="J22" s="8" t="s">
+      <c r="J22" t="s">
         <v>114</v>
       </c>
-      <c r="K22" s="8" t="s">
+      <c r="K22" t="s">
         <v>178</v>
       </c>
       <c r="L22" t="s">
         <v>159</v>
       </c>
-      <c r="M22" s="8" t="s">
+      <c r="M22" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>186</v>
       </c>
@@ -2999,20 +3024,20 @@
       <c r="I23" t="s">
         <v>28</v>
       </c>
-      <c r="J23" s="8" t="s">
+      <c r="J23" t="s">
         <v>188</v>
       </c>
-      <c r="K23" s="8" t="s">
+      <c r="K23" t="s">
         <v>189</v>
       </c>
-      <c r="L23" s="8" t="s">
+      <c r="L23" t="s">
         <v>190</v>
       </c>
-      <c r="M23" s="8" t="s">
+      <c r="M23" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>192</v>
       </c>
@@ -3040,20 +3065,20 @@
       <c r="I24" t="s">
         <v>28</v>
       </c>
-      <c r="J24" s="8" t="s">
+      <c r="J24" t="s">
         <v>188</v>
       </c>
-      <c r="K24" s="8" t="s">
+      <c r="K24" t="s">
         <v>189</v>
       </c>
-      <c r="L24" s="8" t="s">
+      <c r="L24" t="s">
         <v>190</v>
       </c>
-      <c r="M24" s="8" t="s">
+      <c r="M24" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>196</v>
       </c>
@@ -3081,16 +3106,16 @@
       <c r="I25" t="s">
         <v>28</v>
       </c>
-      <c r="J25" s="8" t="s">
+      <c r="J25" t="s">
         <v>197</v>
       </c>
-      <c r="K25" s="8" t="s">
+      <c r="K25" t="s">
         <v>198</v>
       </c>
-      <c r="L25" s="8" t="s">
+      <c r="L25" t="s">
         <v>199</v>
       </c>
-      <c r="M25" s="8" t="s">
+      <c r="M25" t="s">
         <v>200</v>
       </c>
     </row>
@@ -3107,14 +3132,14 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="50" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -3122,7 +3147,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -3130,10 +3155,10 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>41</v>
       </c>
@@ -3141,7 +3166,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>42</v>
       </c>
@@ -3149,10 +3174,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>36</v>
       </c>
@@ -3166,7 +3191,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -3177,7 +3202,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -3191,7 +3216,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>3</v>
       </c>
@@ -3205,7 +3230,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>4</v>
       </c>
@@ -3220,7 +3245,7 @@
       </c>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>5</v>
       </c>
@@ -3234,7 +3259,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>6</v>
       </c>
@@ -3248,7 +3273,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>7</v>
       </c>
@@ -3262,7 +3287,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>8</v>
       </c>
@@ -3276,7 +3301,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>9</v>
       </c>
@@ -3290,7 +3315,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>10</v>
       </c>
@@ -3304,7 +3329,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>11</v>
       </c>
@@ -3318,7 +3343,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Several script descriptions added
</commit_message>
<xml_diff>
--- a/r0 SCRIPTS.xlsx
+++ b/r0 SCRIPTS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://netorg4197135-my.sharepoint.com/personal/will_brown_chip-diagnostics_com/Documents/Documents/Github/cd-alpha/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chipdx/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{56D8781F-64E5-0E4B-96A7-1774F22AB709}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8ED1ED5-020A-4065-AB13-CEE09EEC7460}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E2B063-2821-F54E-8258-18D897B6E7B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4F228711-34F2-CD4A-B88C-4A9EDC5CE2D1}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15500" activeTab="1" xr2:uid="{4F228711-34F2-CD4A-B88C-4A9EDC5CE2D1}"/>
   </bookViews>
   <sheets>
     <sheet name="r0" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="668" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="245">
   <si>
     <t>Sample Flow Rate</t>
   </si>
@@ -651,13 +651,195 @@
   </si>
   <si>
     <t>0 mins</t>
+  </si>
+  <si>
+    <t>ExoT_r0_script_18v0</t>
+  </si>
+  <si>
+    <t>5.5 mL</t>
+  </si>
+  <si>
+    <t>lysate/700</t>
+  </si>
+  <si>
+    <t xml:space="preserve">See QC Checklist_r0-protocol-18v0.xlsx </t>
+  </si>
+  <si>
+    <t>r0-protocol-18v1.json</t>
+  </si>
+  <si>
+    <t>lysate/200+750</t>
+  </si>
+  <si>
+    <t>r0-protocol-16v2.json</t>
+  </si>
+  <si>
+    <t>Western Blot 4 for r0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 mL/hr for 600 uL then 50 mL/hr for remaining </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exact copy of v0_16v2 with modifications for r0 (1.8 mL F-127, 1 hr F-127 incubation via slow flow 0.5 mL @ 0.5 mL/hr) </t>
+  </si>
+  <si>
+    <t>v0-protocol-17v1.json</t>
+  </si>
+  <si>
+    <t>200-800-1000 (600 uL @ 10 mL/hr, remainder @ 50 mL/hr)</t>
+  </si>
+  <si>
+    <t>3 mins (QIAzol - 700 uL)</t>
+  </si>
+  <si>
+    <t>waste/500 @ 50 mL/hr</t>
+  </si>
+  <si>
+    <r>
+      <t>Update 17v0 - change final pull back to pulling chip dry, run all reservoirs to 0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>back off waste during extraction</t>
+    </r>
+  </si>
+  <si>
+    <t>v0-protocol-19v0.json</t>
+  </si>
+  <si>
+    <t>2.5 mL/hr</t>
+  </si>
+  <si>
+    <t>1 mL sample, 2.5 mL/hr small open TENPO</t>
+  </si>
+  <si>
+    <t>6 mins (QIAzol - 700 uL) - VIA 7 mL/hr pull!</t>
+  </si>
+  <si>
+    <t>All to lysate</t>
+  </si>
+  <si>
+    <t>v0-protocol-21v0.json</t>
+  </si>
+  <si>
+    <t>0.5 mL sample, 4.5 mL/hr small open TENPO</t>
+  </si>
+  <si>
+    <t>4.5 mL/hr</t>
+  </si>
+  <si>
+    <t>2 mins (4:48 total with pulls)</t>
+  </si>
+  <si>
+    <t>v0-protocol-19v1_1mL.json</t>
+  </si>
+  <si>
+    <t>v0-protocol-19v1_0.5mL.json</t>
+  </si>
+  <si>
+    <t>v0-protocol-19v2_DEMO.json</t>
+  </si>
+  <si>
+    <t>v0-protocol-21v1.json</t>
+  </si>
+  <si>
+    <t>02:30 (~5m total with pulls)</t>
+  </si>
+  <si>
+    <t>v0-protocol-21v2.json</t>
+  </si>
+  <si>
+    <t>v0-protocol-21v3.json</t>
+  </si>
+  <si>
+    <t>0.5 mL sample, 1.0 mL/hr small open TENPO</t>
+  </si>
+  <si>
+    <t>1.0 mL/hr</t>
+  </si>
+  <si>
+    <r>
+      <t>v0-protocol-21v</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.json</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1.0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> mL sample, 1.0 mL/hr small open TENPO</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1.0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> mL</t>
+    </r>
+  </si>
+  <si>
+    <t>v0-protocol-22v0.json</t>
+  </si>
+  <si>
+    <t>1 mL sample, 1.5 mL/hr small open TENPO</t>
+  </si>
+  <si>
+    <t>1.5 mL/hr</t>
+  </si>
+  <si>
+    <t>RIPA 600 uL; 03:00 15 mL/hr (~5m total with pulls)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -716,8 +898,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -728,6 +925,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
   </fills>
@@ -743,7 +946,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -758,6 +961,22 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1072,34 +1291,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{865254A0-CD44-564E-904D-D988B38D1DFE}">
-  <dimension ref="A1:K35"/>
+  <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="J36" sqref="J36"/>
+      <selection pane="bottomRight" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="49" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.625" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="20.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="20.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1134,7 +1353,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1169,7 +1388,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>104</v>
       </c>
@@ -1204,7 +1423,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -1239,7 +1458,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1274,7 +1493,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1309,7 +1528,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>65</v>
       </c>
@@ -1344,7 +1563,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>66</v>
       </c>
@@ -1379,7 +1598,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>67</v>
       </c>
@@ -1414,7 +1633,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -1449,7 +1668,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>69</v>
       </c>
@@ -1484,7 +1703,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>74</v>
       </c>
@@ -1519,7 +1738,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>77</v>
       </c>
@@ -1554,7 +1773,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>79</v>
       </c>
@@ -1589,7 +1808,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>80</v>
       </c>
@@ -1624,7 +1843,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>82</v>
       </c>
@@ -1656,7 +1875,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>83</v>
       </c>
@@ -1691,7 +1910,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>89</v>
       </c>
@@ -1726,7 +1945,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>90</v>
       </c>
@@ -1761,7 +1980,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>91</v>
       </c>
@@ -1796,7 +2015,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>92</v>
       </c>
@@ -1831,7 +2050,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>94</v>
       </c>
@@ -1866,7 +2085,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>95</v>
       </c>
@@ -1901,7 +2120,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>98</v>
       </c>
@@ -1936,7 +2155,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>100</v>
       </c>
@@ -1971,7 +2190,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>102</v>
       </c>
@@ -2006,7 +2225,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>108</v>
       </c>
@@ -2041,7 +2260,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>147</v>
       </c>
@@ -2076,7 +2295,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>148</v>
       </c>
@@ -2111,7 +2330,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>149</v>
       </c>
@@ -2146,7 +2365,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>150</v>
       </c>
@@ -2181,76 +2400,243 @@
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="34" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B34" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D34" t="s">
-        <v>12</v>
-      </c>
-      <c r="E34" t="s">
-        <v>30</v>
-      </c>
-      <c r="F34" t="s">
+      <c r="D34" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F34" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="G34" t="s">
-        <v>14</v>
-      </c>
-      <c r="H34" t="s">
-        <v>14</v>
-      </c>
-      <c r="I34" t="s">
+      <c r="G34" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H34" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I34" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="J34" t="s">
+      <c r="J34" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="K34" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="K34" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B35" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="C35" t="s">
-        <v>12</v>
-      </c>
-      <c r="D35" t="s">
-        <v>12</v>
-      </c>
-      <c r="E35" t="s">
-        <v>30</v>
-      </c>
-      <c r="F35" t="s">
+      <c r="C35" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F35" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="G35" t="s">
+      <c r="G35" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="H35" t="s">
-        <v>14</v>
-      </c>
-      <c r="I35" t="s">
+      <c r="H35" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="I35" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="J35" t="s">
+      <c r="J35" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="K35" t="s">
-        <v>25</v>
-      </c>
-    </row>
+      <c r="K35" s="10" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="11" t="s">
+        <v>211</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>212</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F38" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H38" s="11" t="s">
+        <v>213</v>
+      </c>
+      <c r="I38" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J38" s="11" t="s">
+        <v>188</v>
+      </c>
+      <c r="K38" s="11" t="s">
+        <v>189</v>
+      </c>
+      <c r="L38" s="11" t="s">
+        <v>190</v>
+      </c>
+      <c r="M38" s="11" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="11" t="s">
+        <v>196</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="C39" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F39" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H39" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="I39" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J39" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="K39" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="L39" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="M39" s="11" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="11" t="s">
+        <v>205</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>202</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E40" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="G40" s="11" t="s">
+        <v>162</v>
+      </c>
+      <c r="H40" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I40" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="J40" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="K40" s="11" t="s">
+        <v>207</v>
+      </c>
+      <c r="L40" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="M40" s="11" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A41" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="C41" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D41" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E41" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F41" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="G41" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="H41" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I41" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="J41" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="K41" s="13" t="s">
+        <v>210</v>
+      </c>
+      <c r="L41" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="M41" s="13"/>
+    </row>
+    <row r="42" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2259,27 +2645,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{789722DC-7BCB-4884-BC3A-D96FA1424135}">
-  <dimension ref="A1:O25"/>
+  <dimension ref="A1:O39"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M26" sqref="M26"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="F1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.875" customWidth="1"/>
-    <col min="2" max="2" width="43.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="34.125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5" customWidth="1"/>
+    <col min="2" max="2" width="43.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="25.5" customWidth="1"/>
     <col min="11" max="11" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="36.375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="36.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>85</v>
       </c>
@@ -2295,7 +2682,7 @@
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
     </row>
-    <row r="3" spans="1:15" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2337,7 +2724,7 @@
       </c>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>86</v>
       </c>
@@ -2372,7 +2759,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>110</v>
       </c>
@@ -2407,7 +2794,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>113</v>
       </c>
@@ -2445,7 +2832,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>116</v>
       </c>
@@ -2480,7 +2867,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>123</v>
       </c>
@@ -2521,7 +2908,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>125</v>
       </c>
@@ -2562,7 +2949,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>127</v>
       </c>
@@ -2603,7 +2990,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>132</v>
       </c>
@@ -2614,12 +3001,12 @@
         <v>133</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>153</v>
       </c>
@@ -2630,7 +3017,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>137</v>
       </c>
@@ -2671,7 +3058,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>138</v>
       </c>
@@ -2712,7 +3099,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>152</v>
       </c>
@@ -2750,7 +3137,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>161</v>
       </c>
@@ -2791,7 +3178,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>163</v>
       </c>
@@ -2832,7 +3219,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>169</v>
       </c>
@@ -2873,7 +3260,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>172</v>
       </c>
@@ -2914,7 +3301,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>173</v>
       </c>
@@ -2955,7 +3342,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>176</v>
       </c>
@@ -2996,7 +3383,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>186</v>
       </c>
@@ -3037,7 +3424,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>192</v>
       </c>
@@ -3078,47 +3465,481 @@
         <v>193</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="25" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="10" t="s">
         <v>196</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="C25" t="s">
-        <v>12</v>
-      </c>
-      <c r="D25" t="s">
-        <v>12</v>
-      </c>
-      <c r="E25" t="s">
-        <v>30</v>
-      </c>
-      <c r="F25" t="s">
+      <c r="C25" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F25" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="G25" t="s">
+      <c r="G25" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H25" t="s">
+      <c r="H25" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I25" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="J25" t="s">
+      <c r="J25" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="K25" t="s">
+      <c r="K25" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="L25" t="s">
+      <c r="L25" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="M25" t="s">
+      <c r="M25" s="10" t="s">
         <v>200</v>
       </c>
     </row>
+    <row r="26" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="C26" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F26" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="G26" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="H26" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="I26" s="11" t="s">
+        <v>216</v>
+      </c>
+      <c r="J26" s="14" t="s">
+        <v>217</v>
+      </c>
+      <c r="K26" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="L26" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="M26" s="11" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="11" t="s">
+        <v>220</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="H27" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I27" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="J27" s="11" t="s">
+        <v>197</v>
+      </c>
+      <c r="K27" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="L27" s="11" t="s">
+        <v>199</v>
+      </c>
+      <c r="M27" s="11"/>
+    </row>
+    <row r="28" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G28" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="H28" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I28" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="J28" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="K28" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="L28" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="M28" s="11"/>
+    </row>
+    <row r="29" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="11" t="s">
+        <v>229</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="G29" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="H29" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I29" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="J29" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="K29" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="L29" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="M29" s="11"/>
+    </row>
+    <row r="30" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="11" t="s">
+        <v>231</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="G30" s="11" t="s">
+        <v>221</v>
+      </c>
+      <c r="H30" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I30" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="J30" s="14" t="s">
+        <v>223</v>
+      </c>
+      <c r="K30" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="L30" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="M30" s="11"/>
+    </row>
+    <row r="31" spans="1:13" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="13" t="s">
+        <v>225</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G31" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="H31" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I31" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="J31" s="15" t="s">
+        <v>228</v>
+      </c>
+      <c r="K31" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="L31" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="M31" s="13"/>
+    </row>
+    <row r="32" spans="1:13" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="13" t="s">
+        <v>232</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F32" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G32" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="H32" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I32" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="J32" s="15" t="s">
+        <v>233</v>
+      </c>
+      <c r="K32" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="L32" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="M32" s="13"/>
+    </row>
+    <row r="33" spans="1:13" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A33" s="13" t="s">
+        <v>234</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>226</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F33" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G33" s="13" t="s">
+        <v>227</v>
+      </c>
+      <c r="H33" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I33" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="J33" s="15" t="s">
+        <v>233</v>
+      </c>
+      <c r="K33" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="L33" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="M33" s="13"/>
+    </row>
+    <row r="34" spans="1:13" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="13" t="s">
+        <v>235</v>
+      </c>
+      <c r="B34" s="13" t="s">
+        <v>236</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F34" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G34" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="H34" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I34" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="J34" s="15" t="s">
+        <v>233</v>
+      </c>
+      <c r="K34" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="L34" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="M34" s="13"/>
+    </row>
+    <row r="35" spans="1:13" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A35" s="13" t="s">
+        <v>238</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>239</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E35" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F35" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="G35" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="H35" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I35" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="J35" s="15" t="s">
+        <v>233</v>
+      </c>
+      <c r="K35" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="L35" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="M35" s="13"/>
+    </row>
+    <row r="36" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>242</v>
+      </c>
+      <c r="C36" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="F36" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="G36" s="11" t="s">
+        <v>243</v>
+      </c>
+      <c r="H36" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I36" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="J36" s="14" t="s">
+        <v>244</v>
+      </c>
+      <c r="K36" s="11" t="s">
+        <v>224</v>
+      </c>
+      <c r="L36" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="M36" s="11"/>
+    </row>
+    <row r="37" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="1:13" s="10" customFormat="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3132,14 +3953,14 @@
       <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="50" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>32</v>
       </c>
@@ -3147,7 +3968,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -3155,10 +3976,10 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>41</v>
       </c>
@@ -3166,7 +3987,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>42</v>
       </c>
@@ -3174,10 +3995,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>36</v>
       </c>
@@ -3191,7 +4012,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -3202,7 +4023,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2</v>
       </c>
@@ -3216,7 +4037,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>3</v>
       </c>
@@ -3230,7 +4051,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>4</v>
       </c>
@@ -3245,7 +4066,7 @@
       </c>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>5</v>
       </c>
@@ -3259,7 +4080,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>6</v>
       </c>
@@ -3273,7 +4094,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>7</v>
       </c>
@@ -3287,7 +4108,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>8</v>
       </c>
@@ -3301,7 +4122,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>9</v>
       </c>
@@ -3315,7 +4136,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>10</v>
       </c>
@@ -3329,7 +4150,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>11</v>
       </c>
@@ -3343,7 +4164,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>12</v>
       </c>

</xml_diff>